<commit_message>
Modify the input parameters to be randomly generated
</commit_message>
<xml_diff>
--- a/UI/getdata/test.xlsx
+++ b/UI/getdata/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7DAF2D-FFA3-4295-A9D5-64EB2322A0D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F250D005-728E-49C5-B759-48352FF42C96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_customer" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>entityType</t>
   </si>
@@ -32,24 +32,9 @@
     <t>salutation</t>
   </si>
   <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
     <t>suffix</t>
   </si>
   <si>
-    <t>fullName</t>
-  </si>
-  <si>
-    <t>default_sort</t>
-  </si>
-  <si>
-    <t>organizationName</t>
-  </si>
-  <si>
     <t>typeOfBusiness</t>
   </si>
   <si>
@@ -59,9 +44,6 @@
     <t>emailType</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>Person</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -107,14 +89,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CfirstName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ClastName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>role</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -138,42 +112,14 @@
     <t>Business</t>
   </si>
   <si>
-    <t>test@qq.com</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>areaCode1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>phone1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>type1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>areaCode2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>phone2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>type2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>areaCode3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>phone3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>type3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -190,30 +136,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>111</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111111</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>222</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2222222</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>333</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>3333333</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Person</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -222,14 +144,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> Trust/Estate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Household</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>County</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -247,10 +161,6 @@
   </si>
   <si>
     <t>D.D.S.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>contact</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -334,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -350,12 +260,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -638,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -650,7 +554,7 @@
     <col min="2" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -669,145 +573,103 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-    </row>
-    <row r="5" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -818,15 +680,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A5BCB2-F6ED-4C63-B189-A41DC03A6A14}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -846,196 +708,82 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="K3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="L3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{D72A9EB0-50A5-440B-A716-F97FD1BE120D}"/>
-    <hyperlink ref="P3" r:id="rId2" xr:uid="{44A9C440-1809-40A0-9C4B-491B2AD0808F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dictionary type parameter get data from database
</commit_message>
<xml_diff>
--- a/UI/getdata/test.xlsx
+++ b/UI/getdata/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F250D005-728E-49C5-B759-48352FF42C96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D249E4-3C27-4979-931B-0ECBC8359D71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>entityType</t>
   </si>
@@ -29,162 +29,170 @@
     <t>entityClass</t>
   </si>
   <si>
+    <t>typeOfBusiness</t>
+  </si>
+  <si>
+    <t>Person</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Individual</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sr.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t>Organization</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Limited Liability Company</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AZ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trust/Estate</t>
+  </si>
+  <si>
+    <t>AK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Person</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sole Proprietor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dr.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sr.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>type1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>type2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>type3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agent</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cell</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fax</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Person</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Government</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>County</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sole Proprietor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dr.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D.D.S.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rev.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Personal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fax</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Office</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>emailType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stateOfIncorporation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>suffix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>salutation</t>
-  </si>
-  <si>
-    <t>suffix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>typeOfBusiness</t>
-  </si>
-  <si>
-    <t>stateOfIncorporation</t>
-  </si>
-  <si>
-    <t>emailType</t>
-  </si>
-  <si>
-    <t>Person</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Individual</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Miss</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sr.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Household</t>
-  </si>
-  <si>
-    <t>Organization</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Company</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Limited Liability Company</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AZ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trust/Estate</t>
-  </si>
-  <si>
-    <t>AK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>role</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Person</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sole Proprietor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dr.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sr.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>type1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>type2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>type3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Agent</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cell</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fax</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Person</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Government</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>County</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sole Proprietor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dr.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>D.D.S.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rev.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CPA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Personal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fax</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Office</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>III</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -545,7 +553,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -562,16 +570,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -584,16 +592,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="4"/>
@@ -602,16 +610,16 @@
     </row>
     <row r="3" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="4"/>
@@ -620,16 +628,16 @@
     </row>
     <row r="4" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="4"/>
@@ -637,35 +645,35 @@
     </row>
     <row r="5" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="4"/>
@@ -683,7 +691,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -696,89 +704,89 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify the common method operator_identifier to support the BAN
</commit_message>
<xml_diff>
--- a/UI/getdata/test.xlsx
+++ b/UI/getdata/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D249E4-3C27-4979-931B-0ECBC8359D71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809B6A59-1E96-44FF-9836-2E294FD0395E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>entityType</t>
   </si>
@@ -193,6 +193,47 @@
   </si>
   <si>
     <t>typeOfBusiness</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clerk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consultant</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accountant</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Company</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Government</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unknown</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Business</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Office</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -223,12 +264,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,9 +287,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -266,12 +304,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,7 +588,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -581,11 +616,21 @@
       <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="L1" s="2"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -603,7 +648,21 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="1"/>
@@ -621,7 +680,21 @@
       <c r="F3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="1"/>
@@ -639,7 +712,21 @@
       <c r="D4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="5"/>
+      <c r="G4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
@@ -656,6 +743,21 @@
       <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -664,6 +766,21 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -675,7 +792,21 @@
       <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
@@ -691,7 +822,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add case for validate customer permission
</commit_message>
<xml_diff>
--- a/UI/getdata/test.xlsx
+++ b/UI/getdata/test.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809B6A59-1E96-44FF-9836-2E294FD0395E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2514DC92-8442-4F9A-A666-9261B21C9033}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="new_customer" sheetId="1" r:id="rId1"/>
-    <sheet name="two_contact" sheetId="2" r:id="rId2"/>
+    <sheet name="account" sheetId="3" r:id="rId1"/>
+    <sheet name="new_customer" sheetId="1" r:id="rId2"/>
+    <sheet name="two_contact" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
   <si>
     <t>entityType</t>
   </si>
@@ -234,6 +235,97 @@
   </si>
   <si>
     <t>Other</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>addressType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stateCode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>identifierName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consultant</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mailing</t>
+  </si>
+  <si>
+    <t>AR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>State Tax ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Internal GLO ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>username</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yan.liu@an-chen.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Lychan@2012 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1925719012@qq.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abc1234%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tangjiu2020@163.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abc1234%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>elena022@163.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>elena011@163.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Master</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Security</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer Read</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -241,7 +333,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +361,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -287,10 +387,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -305,8 +406,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -584,17 +692,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025AD070-23B3-4FFD-850A-4212E2D532A9}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.25" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{72C22386-54A2-45B8-89EB-004B0204B1A5}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C3DF65DA-DD43-4475-943A-2D46BC816BA7}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{83A5F3B5-1412-4429-A28E-7460F7AC3DBF}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{94AAC166-29AA-4EAA-90B0-BB3C3BF3FE7C}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{F30B72D1-48C5-4F0C-A612-F5DFE6A90590}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{3B2562A9-B766-4A19-97B4-E97F5AE58A02}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.125" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="3"/>
+    <col min="2" max="13" width="9" style="3"/>
+    <col min="14" max="14" width="9" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
@@ -817,17 +1017,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A5BCB2-F6ED-4C63-B189-A41DC03A6A14}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -861,8 +1061,17 @@
       <c r="K1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="L1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -890,8 +1099,17 @@
       <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -918,6 +1136,15 @@
       </c>
       <c r="K3" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>